<commit_message>
add required sql statements and fix error in excel file
</commit_message>
<xml_diff>
--- a/backend/servers/apiserver/common/class_lab_test.xlsx
+++ b/backend/servers/apiserver/common/class_lab_test.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="158">
   <si>
     <t xml:space="preserve">Class Attendance List: 2022, 2  Date: 15-JUN-2023 13:01</t>
   </si>
@@ -413,6 +413,9 @@
   </si>
   <si>
     <t xml:space="preserve">YAP WEI LING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YAPW9088</t>
   </si>
   <si>
     <t xml:space="preserve">Class Group: A32</t>
@@ -601,15 +604,15 @@
   </sheetPr>
   <dimension ref="A1:F88"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F30" activeCellId="0" sqref="F30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F70" activeCellId="0" sqref="F70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="43.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="44.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="44.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="2.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="6.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.13"/>
@@ -1738,22 +1741,22 @@
         <v>13</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>75</v>
+        <v>131</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1772,7 +1775,7 @@
         <v>1</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>18</v>
@@ -1781,10 +1784,10 @@
         <v>12</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1792,7 +1795,7 @@
         <v>2</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>18</v>
@@ -1832,7 +1835,7 @@
         <v>4</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>18</v>
@@ -1852,7 +1855,7 @@
         <v>5</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>11</v>
@@ -1864,7 +1867,7 @@
         <v>13</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1872,7 +1875,7 @@
         <v>6</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>11</v>
@@ -1881,10 +1884,10 @@
         <v>12</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1892,7 +1895,7 @@
         <v>7</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>53</v>
@@ -1912,7 +1915,7 @@
         <v>8</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>18</v>
@@ -1924,7 +1927,7 @@
         <v>13</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1932,7 +1935,7 @@
         <v>9</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>11</v>
@@ -1944,7 +1947,7 @@
         <v>13</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1952,7 +1955,7 @@
         <v>10</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>11</v>
@@ -1964,7 +1967,7 @@
         <v>13</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1972,7 +1975,7 @@
         <v>11</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>18</v>
@@ -1984,7 +1987,7 @@
         <v>13</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1992,7 +1995,7 @@
         <v>12</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>11</v>
@@ -2004,7 +2007,7 @@
         <v>13</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2012,7 +2015,7 @@
         <v>13</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>53</v>
@@ -2024,7 +2027,7 @@
         <v>13</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>